<commit_message>
add markdown exec to documents.
</commit_message>
<xml_diff>
--- a/docs/research/compute/gpu_comparison.xlsx
+++ b/docs/research/compute/gpu_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NathanJohnson\PycharmProjects\dandy\docs\research\gpu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NathanJohnson\PycharmProjects\dandy\docs\research\compute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDAF6E55-CA18-4F7A-9DFF-F66A149399ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EFB156-7AD4-43A1-992B-C45061444235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13200" yWindow="3876" windowWidth="23232" windowHeight="16332" xr2:uid="{2738905B-E797-4BE8-AFD6-AC2FA6D44F79}"/>
+    <workbookView xWindow="22944" yWindow="0" windowWidth="23232" windowHeight="16296" xr2:uid="{2738905B-E797-4BE8-AFD6-AC2FA6D44F79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="37">
   <si>
     <t>Brand</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Model</t>
   </si>
   <si>
-    <t>Power</t>
-  </si>
-  <si>
     <t>Nvidia</t>
   </si>
   <si>
@@ -56,21 +53,111 @@
     <t>Price</t>
   </si>
   <si>
-    <t>VRAM</t>
-  </si>
-  <si>
     <t>RTX 4500</t>
   </si>
   <si>
-    <t>Price Per GB</t>
+    <t>RTX 4090</t>
+  </si>
+  <si>
+    <t>RTX 3090</t>
+  </si>
+  <si>
+    <t>RTX 5090</t>
+  </si>
+  <si>
+    <t>RTX 4000</t>
+  </si>
+  <si>
+    <t>RTX 3000</t>
+  </si>
+  <si>
+    <t>RTX 2000</t>
+  </si>
+  <si>
+    <t>RXT 1000</t>
+  </si>
+  <si>
+    <t>TF16</t>
+  </si>
+  <si>
+    <t>vrGB</t>
+  </si>
+  <si>
+    <t>$vrGB</t>
+  </si>
+  <si>
+    <t>$vrGBPS</t>
+  </si>
+  <si>
+    <t>vrGBPS</t>
+  </si>
+  <si>
+    <t>$OTPS8BQ4</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Perf</t>
+  </si>
+  <si>
+    <t>OTPDAY</t>
+  </si>
+  <si>
+    <t>WPOT</t>
+  </si>
+  <si>
+    <t>Intel</t>
+  </si>
+  <si>
+    <t>B580</t>
+  </si>
+  <si>
+    <t>B570</t>
+  </si>
+  <si>
+    <t>A770</t>
+  </si>
+  <si>
+    <t>pWATT*</t>
+  </si>
+  <si>
+    <t>OTPS8BQ4*</t>
+  </si>
+  <si>
+    <t>$TF16</t>
+  </si>
+  <si>
+    <t>Specs</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>7900XT</t>
+  </si>
+  <si>
+    <t>9070XT</t>
+  </si>
+  <si>
+    <t>W7900</t>
+  </si>
+  <si>
+    <t>W7800</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -105,19 +192,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -451,20 +553,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2983A6D-D6E0-4279-951B-AB7DBB033190}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="9" width="13.6640625" style="5" customWidth="1"/>
+    <col min="10" max="14" width="13.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" style="4" customWidth="1"/>
+    <col min="18" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -472,100 +582,920 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4000</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="5">
+        <v>32</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1790</v>
+      </c>
+      <c r="G2" s="5">
+        <v>104.8</v>
+      </c>
+      <c r="H2" s="5">
+        <v>500</v>
+      </c>
+      <c r="I2" s="5">
+        <v>180</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2">
+        <f>$C2/E2</f>
+        <v>125</v>
+      </c>
+      <c r="L2" s="2">
+        <f>$C2/F2</f>
+        <v>2.2346368715083798</v>
+      </c>
+      <c r="M2" s="2">
+        <f>$C2/G2</f>
+        <v>38.167938931297712</v>
+      </c>
+      <c r="N2" s="2">
+        <f>$C2/I3</f>
+        <v>28.571428571428573</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" s="10">
+        <f>I2*86400</f>
+        <v>15552000</v>
+      </c>
+      <c r="Q2" s="4">
+        <f>H2/I2</f>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="R2" s="6"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3000</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5">
+        <v>24</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1010</v>
+      </c>
+      <c r="G3" s="5">
+        <v>82.6</v>
+      </c>
+      <c r="H3" s="5">
+        <v>450</v>
+      </c>
+      <c r="I3" s="5">
+        <v>140</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2">
+        <f>$C3/E3</f>
+        <v>125</v>
+      </c>
+      <c r="L3" s="2">
+        <f>$C3/F3</f>
+        <v>2.9702970297029703</v>
+      </c>
+      <c r="M3" s="2">
+        <f>$C3/G3</f>
+        <v>36.319612590799032</v>
+      </c>
+      <c r="N3" s="2">
+        <f>$C3/I3</f>
+        <v>21.428571428571427</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="10">
+        <f t="shared" ref="P3:P10" si="0">I3*86400</f>
+        <v>12096000</v>
+      </c>
+      <c r="Q3" s="4">
+        <f t="shared" ref="Q3:Q10" si="1">H3/I3</f>
+        <v>3.2142857142857144</v>
+      </c>
+      <c r="R3" s="6"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="5">
+        <v>24</v>
+      </c>
+      <c r="F4" s="5">
+        <v>936</v>
+      </c>
+      <c r="G4" s="5">
+        <v>35.6</v>
+      </c>
+      <c r="H4" s="5">
+        <v>350</v>
+      </c>
+      <c r="I4" s="5">
+        <v>120</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="2">
+        <f>$C4/E4</f>
+        <v>62.5</v>
+      </c>
+      <c r="L4" s="2">
+        <f>$C4/F4</f>
+        <v>1.6025641025641026</v>
+      </c>
+      <c r="M4" s="2">
+        <f>$C4/G4</f>
+        <v>42.134831460674157</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" ref="N4:N10" si="2">$C4/I4</f>
+        <v>12.5</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" s="10">
+        <f t="shared" si="0"/>
+        <v>10368000</v>
+      </c>
+      <c r="Q4" s="4">
+        <f t="shared" si="1"/>
+        <v>2.9166666666666665</v>
+      </c>
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="5">
+        <v>48</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2">
+        <f>$C5/E5</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="e">
+        <f>$C5/F5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" s="2" t="e">
+        <f>$C5/G5</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N5" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R5" s="6"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>300</v>
-      </c>
-      <c r="D2" s="1">
-        <v>8000</v>
-      </c>
-      <c r="E2">
-        <v>48</v>
-      </c>
-      <c r="F2" s="2">
-        <f>D2/E2</f>
-        <v>166.66666666666666</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>300</v>
-      </c>
-      <c r="D3" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E3">
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5">
         <v>24</v>
       </c>
-      <c r="F3" s="2">
-        <f>D3/E3</f>
-        <v>166.66666666666666</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>300</v>
-      </c>
-      <c r="D4" s="1">
-        <v>8000</v>
-      </c>
-      <c r="E4">
-        <v>48</v>
-      </c>
-      <c r="F4" s="2">
-        <f>D4/E4</f>
-        <v>166.66666666666666</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>300</v>
-      </c>
-      <c r="D5" s="1">
-        <v>4000</v>
-      </c>
-      <c r="E5">
+      <c r="J6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="2">
+        <f>$C6/E6</f>
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="e">
+        <f>$C6/F6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M6" s="2" t="e">
+        <f>$C6/G6</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N6" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R6" s="6"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="2" t="e">
+        <f>$C7/E7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L7" s="2" t="e">
+        <f>$C7/F7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="2" t="e">
+        <f>$C7/G7</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N7" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R7" s="6"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="2" t="e">
+        <f>$C8/E8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L8" s="2" t="e">
+        <f>$C8/F8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="2" t="e">
+        <f>$C8/G8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R8" s="6"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="2" t="e">
+        <f>$C9/E9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L9" s="2" t="e">
+        <f>$C9/F9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="2" t="e">
+        <f>$C9/G9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R9" s="6"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="2" t="e">
+        <f>$C10/E10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L10" s="2" t="e">
+        <f>$C10/F10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M10" s="2" t="e">
+        <f>$C10/G10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N10" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="4" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R10" s="6"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="2">
-        <f>D5/E5</f>
-        <v>166.66666666666666</v>
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="2" t="e">
+        <f t="shared" ref="K11:K13" si="3">$C11/E11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L11" s="2" t="e">
+        <f t="shared" ref="L11:L13" si="4">$C11/F11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="2" t="e">
+        <f t="shared" ref="M11:M13" si="5">$C11/G11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N11" s="2" t="e">
+        <f t="shared" ref="N11:N13" si="6">$C11/I11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" s="10">
+        <f t="shared" ref="P11:P13" si="7">I11*86400</f>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="4" t="e">
+        <f t="shared" ref="Q11:Q13" si="8">H11/I11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R11" s="6"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="2" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L12" s="2" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" s="2" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N12" s="2" t="e">
+        <f t="shared" si="6"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12" s="10">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="4" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R12" s="6"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="1">
+        <v>500</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="5">
+        <v>16</v>
+      </c>
+      <c r="F13" s="5">
+        <v>512</v>
+      </c>
+      <c r="G13" s="5">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="H13" s="5">
+        <v>225</v>
+      </c>
+      <c r="I13" s="5">
+        <v>69</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>31.25</v>
+      </c>
+      <c r="L13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.9765625</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="5"/>
+        <v>12.722646310432571</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="6"/>
+        <v>7.2463768115942031</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P13" s="10">
+        <f t="shared" si="7"/>
+        <v>5961600</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="8"/>
+        <v>3.2608695652173911</v>
+      </c>
+      <c r="R13" s="6"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="2" t="e">
+        <f t="shared" ref="K14:K19" si="9">$C14/E14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L14" s="2" t="e">
+        <f t="shared" ref="L14:L19" si="10">$C14/F14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M14" s="2" t="e">
+        <f t="shared" ref="M14:M19" si="11">$C14/G14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N14" s="2" t="e">
+        <f t="shared" ref="N14:N19" si="12">$C14/I14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P14" s="10">
+        <f t="shared" ref="P14:P19" si="13">I14*86400</f>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="4" t="e">
+        <f t="shared" ref="Q14:Q19" si="14">H14/I14</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3">
+        <v>9070</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="2" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L15" s="2" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M15" s="2" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" s="2" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P15" s="10">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="2" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L16" s="2" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M16" s="2" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N16" s="2" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" s="10">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="4" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="2" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="2" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M17" s="2" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N17" s="2" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P17" s="10">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3">
+        <v>7800</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="2" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L18" s="2" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M18" s="2" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" s="2" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P18" s="10">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="4" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="2" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L19" s="2" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M19" s="2" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" s="2" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P19" s="10">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="4" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
llm map refactor and retry processing.
</commit_message>
<xml_diff>
--- a/docs/research/compute/gpu_comparison.xlsx
+++ b/docs/research/compute/gpu_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NathanJohnson\PycharmProjects\dandy\docs\research\compute\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{025BB0BC-066D-4E6C-9E1B-C05EA364A471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE078AAE-0FF4-4D3D-974F-40839A477869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9036" yWindow="3744" windowWidth="34560" windowHeight="18600" xr2:uid="{2738905B-E797-4BE8-AFD6-AC2FA6D44F79}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="23316" windowHeight="25296" xr2:uid="{2738905B-E797-4BE8-AFD6-AC2FA6D44F79}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="54">
   <si>
     <t>Brand</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>RTX 5000 Ada</t>
+  </si>
+  <si>
+    <t>A40 Ampere</t>
+  </si>
+  <si>
+    <t>L40 Ada</t>
   </si>
 </sst>
 </file>
@@ -656,13 +662,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2983A6D-D6E0-4279-951B-AB7DBB033190}">
-  <dimension ref="A1:Y26"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomRight" activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,15 +805,15 @@
         <v>12</v>
       </c>
       <c r="L2" s="2">
-        <f t="shared" ref="L2:L11" si="0">$C2/F2</f>
+        <f t="shared" ref="L2:L13" si="0">$C2/F2</f>
         <v>250</v>
       </c>
       <c r="M2" s="2">
-        <f t="shared" ref="M2:M11" si="1">$C2/G2</f>
+        <f t="shared" ref="M2:M13" si="1">$C2/G2</f>
         <v>4.4692737430167595</v>
       </c>
       <c r="N2" s="2">
-        <f t="shared" ref="N2:N11" si="2">$C2/H2</f>
+        <f t="shared" ref="N2:N13" si="2">$C2/H2</f>
         <v>76.335877862595424</v>
       </c>
       <c r="O2" s="2">
@@ -849,7 +855,7 @@
         <v>113529.59999999999</v>
       </c>
       <c r="Y2" s="1">
-        <f t="shared" ref="Y2:Y26" si="3">X2/365/24/60</f>
+        <f t="shared" ref="Y2:Y28" si="3">X2/365/24/60</f>
         <v>0.216</v>
       </c>
     </row>
@@ -918,15 +924,15 @@
         <v>12</v>
       </c>
       <c r="T3" s="1">
-        <f t="shared" ref="T3:T22" si="6">Q3/1000000 *2 * 365</f>
+        <f t="shared" ref="T3:T24" si="6">Q3/1000000 *2 * 365</f>
         <v>8830.08</v>
       </c>
       <c r="U3" s="1">
-        <f t="shared" ref="U3:W23" si="7">T3/365/24/60</f>
+        <f t="shared" ref="U3:W25" si="7">T3/365/24/60</f>
         <v>1.6799999999999999E-2</v>
       </c>
       <c r="V3" s="1">
-        <f t="shared" ref="V3:V22" si="8">Q3/1000000 *4 * 365</f>
+        <f t="shared" ref="V3:V24" si="8">Q3/1000000 *4 * 365</f>
         <v>17660.16</v>
       </c>
       <c r="W3" s="1">
@@ -934,7 +940,7 @@
         <v>3.3599999999999998E-2</v>
       </c>
       <c r="X3" s="1">
-        <f t="shared" ref="X3:X22" si="9">Q3/1000000 *20 * 365</f>
+        <f t="shared" ref="X3:X24" si="9">Q3/1000000 *20 * 365</f>
         <v>88300.800000000003</v>
       </c>
       <c r="Y3" s="1">
@@ -1626,165 +1632,156 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="C12" s="1">
-        <v>500</v>
+        <v>11000</v>
       </c>
       <c r="D12" s="11">
-        <v>1</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F12" s="5">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="G12" s="5">
-        <v>456</v>
+        <v>695</v>
       </c>
       <c r="H12" s="5">
-        <v>27.3</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>12</v>
+        <v>37.42</v>
+      </c>
+      <c r="I12" s="5">
+        <v>300</v>
+      </c>
+      <c r="J12" s="5">
+        <v>90</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" ref="L12:N14" si="11">$C12/F12</f>
-        <v>41.666666666666664</v>
+        <f t="shared" si="0"/>
+        <v>229.16666666666666</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="11"/>
-        <v>1.0964912280701755</v>
+        <f t="shared" si="1"/>
+        <v>15.827338129496402</v>
       </c>
       <c r="N12" s="2">
-        <f t="shared" si="11"/>
-        <v>18.315018315018314</v>
-      </c>
-      <c r="O12" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>293.96044895777658</v>
+      </c>
+      <c r="O12" s="2">
         <f>$C12/J12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="7" t="s">
-        <v>12</v>
+        <v>122.22222222222223</v>
       </c>
       <c r="Q12" s="6">
         <f>J12*86400</f>
-        <v>0</v>
-      </c>
-      <c r="R12" s="4" t="e">
+        <v>7776000</v>
+      </c>
+      <c r="R12" s="4">
         <f>I12/J12</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S12" s="7" t="s">
-        <v>12</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="T12" s="1">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>Q12/1000000 *2 * 365</f>
+        <v>5676.48</v>
       </c>
       <c r="U12" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>T12/365/24/60</f>
+        <v>1.0800000000000001E-2</v>
       </c>
       <c r="V12" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f>Q12/1000000 *4 * 365</f>
+        <v>11352.96</v>
       </c>
       <c r="W12" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>V12/365/24/60</f>
+        <v>2.1600000000000001E-2</v>
       </c>
       <c r="X12" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>Q12/1000000 *20 * 365</f>
+        <v>56764.799999999996</v>
       </c>
       <c r="Y12" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="Y12:Y13" si="11">X12/365/24/60</f>
+        <v>0.108</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="C13" s="1">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="D13" s="11">
-        <v>1</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F13" s="5">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="G13" s="5">
-        <v>360</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>12</v>
+        <v>864</v>
+      </c>
+      <c r="H13" s="5">
+        <v>90</v>
+      </c>
+      <c r="I13" s="5">
+        <v>300</v>
+      </c>
+      <c r="J13" s="5">
+        <v>105</v>
       </c>
       <c r="L13" s="2">
-        <f t="shared" si="11"/>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>208.33333333333334</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" si="11"/>
-        <v>1.3888888888888888</v>
-      </c>
-      <c r="N13" s="2" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O13" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>11.574074074074074</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>111.11111111111111</v>
+      </c>
+      <c r="O13" s="2">
         <f>$C13/J13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>12</v>
+        <v>95.238095238095241</v>
       </c>
       <c r="Q13" s="6">
         <f>J13*86400</f>
-        <v>0</v>
-      </c>
-      <c r="R13" s="4" t="e">
+        <v>9072000</v>
+      </c>
+      <c r="R13" s="4">
         <f>I13/J13</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>12</v>
+        <v>2.8571428571428572</v>
       </c>
       <c r="T13" s="1">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f>Q13/1000000 *2 * 365</f>
+        <v>6622.5599999999995</v>
       </c>
       <c r="U13" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>T13/365/24/60</f>
+        <v>1.2599999999999998E-2</v>
       </c>
       <c r="V13" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
+        <f>Q13/1000000 *4 * 365</f>
+        <v>13245.119999999999</v>
       </c>
       <c r="W13" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>V13/365/24/60</f>
+        <v>2.5199999999999997E-2</v>
       </c>
       <c r="X13" s="1">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f>Q13/1000000 *20 * 365</f>
+        <v>66225.600000000006</v>
       </c>
       <c r="Y13" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>0.12600000000000003</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.3">
@@ -1792,7 +1789,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1">
         <v>500</v>
@@ -1804,253 +1801,250 @@
         <v>12</v>
       </c>
       <c r="F14" s="5">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G14" s="5">
-        <v>512</v>
+        <v>456</v>
       </c>
       <c r="H14" s="5">
-        <v>39.299999999999997</v>
-      </c>
-      <c r="I14" s="5">
-        <v>225</v>
-      </c>
-      <c r="J14" s="5">
-        <v>69</v>
+        <v>27.3</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="L14" s="2">
-        <f t="shared" si="11"/>
-        <v>31.25</v>
+        <f t="shared" ref="L14:N16" si="12">$C14/F14</f>
+        <v>41.666666666666664</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" si="11"/>
-        <v>0.9765625</v>
+        <f t="shared" si="12"/>
+        <v>1.0964912280701755</v>
       </c>
       <c r="N14" s="2">
-        <f t="shared" si="11"/>
-        <v>12.722646310432571</v>
-      </c>
-      <c r="O14" s="2">
+        <f t="shared" si="12"/>
+        <v>18.315018315018314</v>
+      </c>
+      <c r="O14" s="2" t="e">
         <f>$C14/J14</f>
-        <v>7.2463768115942031</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="P14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q14" s="6">
         <f>J14*86400</f>
-        <v>5961600</v>
-      </c>
-      <c r="R14" s="4">
+        <v>0</v>
+      </c>
+      <c r="R14" s="4" t="e">
         <f>I14/J14</f>
-        <v>3.2608695652173911</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="S14" s="7" t="s">
         <v>12</v>
       </c>
       <c r="T14" s="1">
         <f t="shared" si="6"/>
-        <v>4351.9679999999998</v>
+        <v>0</v>
       </c>
       <c r="U14" s="1">
         <f t="shared" si="7"/>
-        <v>8.2799999999999992E-3</v>
+        <v>0</v>
       </c>
       <c r="V14" s="1">
         <f t="shared" si="8"/>
-        <v>8703.9359999999997</v>
+        <v>0</v>
       </c>
       <c r="W14" s="1">
         <f t="shared" si="7"/>
-        <v>1.6559999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="X14" s="1">
         <f t="shared" si="9"/>
-        <v>43519.68</v>
+        <v>0</v>
       </c>
       <c r="Y14" s="1">
         <f t="shared" si="3"/>
-        <v>8.2799999999999999E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1">
-        <v>1800</v>
+        <v>500</v>
       </c>
       <c r="D15" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F15" s="5">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G15" s="5">
-        <v>960</v>
-      </c>
-      <c r="H15" s="5">
-        <v>122.8</v>
-      </c>
-      <c r="I15" s="5">
-        <v>300</v>
-      </c>
-      <c r="J15" s="5">
-        <v>125</v>
+        <v>360</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" ref="L15:L22" si="12">$C15/F15</f>
-        <v>75</v>
+        <f t="shared" si="12"/>
+        <v>50</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" ref="M15:M22" si="13">$C15/G15</f>
-        <v>1.875</v>
-      </c>
-      <c r="N15" s="2">
-        <f t="shared" ref="N15:N22" si="14">$C15/H15</f>
-        <v>14.65798045602606</v>
-      </c>
-      <c r="O15" s="2">
-        <f t="shared" ref="O15:O22" si="15">$C15/J15</f>
-        <v>14.4</v>
+        <f t="shared" si="12"/>
+        <v>1.3888888888888888</v>
+      </c>
+      <c r="N15" s="2" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" s="2" t="e">
+        <f>$C15/J15</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="P15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q15" s="6">
-        <f t="shared" ref="Q15:Q21" si="16">J15*86400</f>
-        <v>10800000</v>
-      </c>
-      <c r="R15" s="4">
-        <f t="shared" ref="R15:R21" si="17">I15/J15</f>
-        <v>2.4</v>
+        <f>J15*86400</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="4" t="e">
+        <f>I15/J15</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="S15" s="7" t="s">
         <v>12</v>
       </c>
       <c r="T15" s="1">
         <f t="shared" si="6"/>
-        <v>7884.0000000000009</v>
+        <v>0</v>
       </c>
       <c r="U15" s="1">
         <f t="shared" si="7"/>
-        <v>1.5000000000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="V15" s="1">
         <f t="shared" si="8"/>
-        <v>15768.000000000002</v>
+        <v>0</v>
       </c>
       <c r="W15" s="1">
         <f t="shared" si="7"/>
-        <v>3.0000000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="X15" s="1">
         <f t="shared" si="9"/>
-        <v>78840</v>
+        <v>0</v>
       </c>
       <c r="Y15" s="1">
         <f t="shared" si="3"/>
-        <v>0.15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
-        <v>1100</v>
+        <v>500</v>
       </c>
       <c r="D16" s="11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="5">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="G16" s="5">
+        <v>512</v>
+      </c>
+      <c r="H16" s="5">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="I16" s="5">
+        <v>225</v>
+      </c>
+      <c r="J16" s="5">
+        <v>69</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="L16" s="2">
-        <f>$C16/F16</f>
-        <v>55</v>
-      </c>
-      <c r="M16" s="2" t="e">
-        <f>$C16/G16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" s="2" t="e">
-        <f>$C16/H16</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="2" t="e">
+        <f t="shared" si="12"/>
+        <v>31.25</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="12"/>
+        <v>0.9765625</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="12"/>
+        <v>12.722646310432571</v>
+      </c>
+      <c r="O16" s="2">
         <f>$C16/J16</f>
-        <v>#DIV/0!</v>
+        <v>7.2463768115942031</v>
       </c>
       <c r="P16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q16" s="6">
         <f>J16*86400</f>
-        <v>0</v>
-      </c>
-      <c r="R16" s="4" t="e">
+        <v>5961600</v>
+      </c>
+      <c r="R16" s="4">
         <f>I16/J16</f>
-        <v>#DIV/0!</v>
+        <v>3.2608695652173911</v>
       </c>
       <c r="S16" s="7" t="s">
         <v>12</v>
       </c>
       <c r="T16" s="1">
-        <f>Q16/1000000 *2 * 365</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>4351.9679999999998</v>
       </c>
       <c r="U16" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>8.2799999999999992E-3</v>
       </c>
       <c r="V16" s="1">
-        <f>Q16/1000000 *4 * 365</f>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>8703.9359999999997</v>
       </c>
       <c r="W16" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.6559999999999998E-2</v>
       </c>
       <c r="X16" s="1">
-        <f>Q16/1000000 *20 * 365</f>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>43519.68</v>
       </c>
       <c r="Y16" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8.2799999999999999E-2</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="3">
-        <v>9070</v>
+      <c r="B17" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C17" s="1">
-        <v>950</v>
+        <v>1800</v>
       </c>
       <c r="D17" s="11">
         <v>2</v>
@@ -2059,64 +2053,76 @@
         <v>12</v>
       </c>
       <c r="F17" s="5">
-        <v>12</v>
+        <v>24</v>
+      </c>
+      <c r="G17" s="5">
+        <v>960</v>
+      </c>
+      <c r="H17" s="5">
+        <v>122.8</v>
+      </c>
+      <c r="I17" s="5">
+        <v>300</v>
+      </c>
+      <c r="J17" s="5">
+        <v>125</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>12</v>
       </c>
       <c r="L17" s="2">
-        <f t="shared" si="12"/>
-        <v>79.166666666666671</v>
-      </c>
-      <c r="M17" s="2" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N17" s="2" t="e">
-        <f t="shared" si="14"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O17" s="2" t="e">
-        <f t="shared" si="15"/>
-        <v>#DIV/0!</v>
+        <f t="shared" ref="L17:L24" si="13">$C17/F17</f>
+        <v>75</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" ref="M17:M24" si="14">$C17/G17</f>
+        <v>1.875</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" ref="N17:N24" si="15">$C17/H17</f>
+        <v>14.65798045602606</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" ref="O17:O24" si="16">$C17/J17</f>
+        <v>14.4</v>
       </c>
       <c r="P17" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q17" s="6">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="R17" s="4" t="e">
-        <f t="shared" si="17"/>
-        <v>#DIV/0!</v>
+        <f t="shared" ref="Q17:Q23" si="17">J17*86400</f>
+        <v>10800000</v>
+      </c>
+      <c r="R17" s="4">
+        <f t="shared" ref="R17:R23" si="18">I17/J17</f>
+        <v>2.4</v>
       </c>
       <c r="S17" s="7" t="s">
         <v>12</v>
       </c>
       <c r="T17" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>7884.0000000000009</v>
       </c>
       <c r="U17" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1.5000000000000001E-2</v>
       </c>
       <c r="V17" s="1">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>15768.000000000002</v>
       </c>
       <c r="W17" s="1">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>3.0000000000000002E-2</v>
       </c>
       <c r="X17" s="1">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>78840</v>
       </c>
       <c r="Y17" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
@@ -2124,7 +2130,7 @@
         <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1">
         <v>1100</v>
@@ -2136,43 +2142,43 @@
         <v>12</v>
       </c>
       <c r="F18" s="5">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="12"/>
-        <v>68.75</v>
+        <f>$C18/F18</f>
+        <v>55</v>
       </c>
       <c r="M18" s="2" t="e">
-        <f t="shared" si="13"/>
+        <f>$C18/G18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N18" s="2" t="e">
-        <f t="shared" si="14"/>
+        <f>$C18/H18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="O18" s="2" t="e">
-        <f t="shared" si="15"/>
+        <f>$C18/J18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="P18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q18" s="6">
-        <f t="shared" si="16"/>
+        <f>J18*86400</f>
         <v>0</v>
       </c>
       <c r="R18" s="4" t="e">
-        <f t="shared" si="17"/>
+        <f>I18/J18</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="T18" s="1">
-        <f t="shared" si="6"/>
+        <f>Q18/1000000 *2 * 365</f>
         <v>0</v>
       </c>
       <c r="U18" s="1">
@@ -2180,7 +2186,7 @@
         <v>0</v>
       </c>
       <c r="V18" s="1">
-        <f t="shared" si="8"/>
+        <f>Q18/1000000 *4 * 365</f>
         <v>0</v>
       </c>
       <c r="W18" s="1">
@@ -2188,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="X18" s="1">
-        <f t="shared" si="9"/>
+        <f>Q18/1000000 *20 * 365</f>
         <v>0</v>
       </c>
       <c r="Y18" s="1">
@@ -2200,11 +2206,11 @@
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>27</v>
+      <c r="B19" s="3">
+        <v>9070</v>
       </c>
       <c r="C19" s="1">
-        <v>5000</v>
+        <v>950</v>
       </c>
       <c r="D19" s="11">
         <v>2</v>
@@ -2213,36 +2219,36 @@
         <v>12</v>
       </c>
       <c r="F19" s="5">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>12</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="12"/>
-        <v>104.16666666666667</v>
+        <f t="shared" si="13"/>
+        <v>79.166666666666671</v>
       </c>
       <c r="M19" s="2" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N19" s="2" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O19" s="2" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P19" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q19" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R19" s="4" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S19" s="7" t="s">
@@ -2278,10 +2284,10 @@
         <v>24</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1">
-        <v>800</v>
+        <v>1100</v>
       </c>
       <c r="D20" s="11">
         <v>2</v>
@@ -2296,30 +2302,30 @@
         <v>12</v>
       </c>
       <c r="L20" s="2">
-        <f t="shared" si="12"/>
-        <v>50</v>
+        <f t="shared" si="13"/>
+        <v>68.75</v>
       </c>
       <c r="M20" s="2" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N20" s="2" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O20" s="2" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q20" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R20" s="4" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S20" s="7" t="s">
@@ -2355,7 +2361,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="1">
         <v>5000</v>
@@ -2367,36 +2373,36 @@
         <v>12</v>
       </c>
       <c r="F21" s="5">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="12"/>
-        <v>156.25</v>
+        <f t="shared" si="13"/>
+        <v>104.16666666666667</v>
       </c>
       <c r="M21" s="2" t="e">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>#DIV/0!</v>
       </c>
       <c r="N21" s="2" t="e">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O21" s="2" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="Q21" s="6">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="R21" s="4" t="e">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S21" s="7" t="s">
@@ -2429,336 +2435,344 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1">
-        <v>9500</v>
+        <v>800</v>
       </c>
       <c r="D22" s="11">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F22" s="5">
-        <v>512</v>
-      </c>
-      <c r="G22" s="5">
-        <v>819</v>
-      </c>
-      <c r="H22" s="5">
-        <v>114</v>
-      </c>
-      <c r="I22" s="5">
-        <v>300</v>
-      </c>
-      <c r="J22" s="5">
-        <v>80</v>
+        <v>16</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="L22" s="2">
-        <f t="shared" si="12"/>
-        <v>18.5546875</v>
-      </c>
-      <c r="M22" s="2">
         <f t="shared" si="13"/>
-        <v>11.599511599511599</v>
-      </c>
-      <c r="N22" s="2">
+        <v>50</v>
+      </c>
+      <c r="M22" s="2" t="e">
         <f t="shared" si="14"/>
-        <v>83.333333333333329</v>
-      </c>
-      <c r="O22" s="2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N22" s="2" t="e">
         <f t="shared" si="15"/>
-        <v>118.75</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" s="2" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="Q22" s="6">
-        <f>J22*86400</f>
-        <v>6912000</v>
-      </c>
-      <c r="R22" s="4">
-        <f>I22/J22</f>
-        <v>3.75</v>
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R22" s="4" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="T22" s="1">
         <f t="shared" si="6"/>
-        <v>5045.76</v>
+        <v>0</v>
       </c>
       <c r="U22" s="1">
         <f t="shared" si="7"/>
-        <v>9.5999999999999992E-3</v>
+        <v>0</v>
       </c>
       <c r="V22" s="1">
         <f t="shared" si="8"/>
-        <v>10091.52</v>
+        <v>0</v>
       </c>
       <c r="W22" s="1">
         <f t="shared" si="7"/>
-        <v>1.9199999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="X22" s="1">
         <f t="shared" si="9"/>
-        <v>50457.600000000006</v>
+        <v>0</v>
       </c>
       <c r="Y22" s="1">
         <f t="shared" si="3"/>
-        <v>9.6000000000000016E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5000</v>
+      </c>
+      <c r="D23" s="11">
+        <v>2</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="5">
         <v>32</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="1">
-        <v>7100</v>
-      </c>
-      <c r="D23" s="11">
-        <v>3</v>
-      </c>
-      <c r="F23" s="5">
-        <v>256</v>
-      </c>
-      <c r="G23" s="5">
-        <v>819</v>
-      </c>
-      <c r="H23" s="5">
-        <v>114</v>
-      </c>
-      <c r="I23" s="5">
-        <v>300</v>
-      </c>
-      <c r="J23" s="5">
-        <v>80</v>
+      <c r="K23" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" ref="L23:N26" si="18">$C23/F23</f>
-        <v>27.734375</v>
-      </c>
-      <c r="M23" s="2">
+        <f t="shared" si="13"/>
+        <v>156.25</v>
+      </c>
+      <c r="M23" s="2" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N23" s="2" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O23" s="2" t="e">
+        <f t="shared" si="16"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q23" s="6">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="R23" s="4" t="e">
         <f t="shared" si="18"/>
-        <v>8.6691086691086685</v>
-      </c>
-      <c r="N23" s="2">
-        <f t="shared" si="18"/>
-        <v>62.280701754385966</v>
-      </c>
-      <c r="O23" s="2">
-        <f>$C23/J23</f>
-        <v>88.75</v>
-      </c>
-      <c r="Q23" s="6">
-        <f>J23*86400</f>
-        <v>6912000</v>
-      </c>
-      <c r="R23" s="4">
-        <f>I23/J23</f>
-        <v>3.75</v>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="T23" s="1">
-        <f>Q23/1000000 *2 * 365</f>
-        <v>5045.76</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="U23" s="1">
         <f t="shared" si="7"/>
-        <v>9.5999999999999992E-3</v>
+        <v>0</v>
       </c>
       <c r="V23" s="1">
-        <f>Q23/1000000 *4 * 365</f>
-        <v>10091.52</v>
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
       <c r="W23" s="1">
         <f t="shared" si="7"/>
-        <v>1.9199999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="X23" s="1">
-        <f>Q23/1000000 *20 * 365</f>
-        <v>50457.600000000006</v>
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="Y23" s="1">
         <f t="shared" si="3"/>
-        <v>9.6000000000000016E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C24" s="1">
-        <v>1500</v>
+        <v>9500</v>
       </c>
       <c r="D24" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F24" s="5">
-        <v>28</v>
+        <v>512</v>
       </c>
       <c r="G24" s="5">
-        <v>512</v>
+        <v>819</v>
+      </c>
+      <c r="H24" s="5">
+        <v>114</v>
       </c>
       <c r="I24" s="5">
         <v>300</v>
       </c>
+      <c r="J24" s="5">
+        <v>80</v>
+      </c>
       <c r="L24" s="2">
-        <f t="shared" si="18"/>
-        <v>53.571428571428569</v>
+        <f t="shared" si="13"/>
+        <v>18.5546875</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" si="18"/>
-        <v>2.9296875</v>
-      </c>
-      <c r="N24" s="2" t="e">
-        <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O24" s="2" t="e">
-        <f>$C24/J24</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="14"/>
+        <v>11.599511599511599</v>
+      </c>
+      <c r="N24" s="2">
+        <f t="shared" si="15"/>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="O24" s="2">
+        <f t="shared" si="16"/>
+        <v>118.75</v>
       </c>
       <c r="Q24" s="6">
         <f>J24*86400</f>
-        <v>0</v>
-      </c>
-      <c r="R24" s="4" t="e">
+        <v>6912000</v>
+      </c>
+      <c r="R24" s="4">
         <f>I24/J24</f>
-        <v>#DIV/0!</v>
+        <v>3.75</v>
       </c>
       <c r="T24" s="1">
-        <f>Q24/1000000 *2 * 365</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>5045.76</v>
       </c>
       <c r="U24" s="1">
-        <f>T24/365/24/60</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>9.5999999999999992E-3</v>
       </c>
       <c r="V24" s="1">
-        <f>Q24/1000000 *4 * 365</f>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>10091.52</v>
       </c>
       <c r="W24" s="1">
-        <f>V24/365/24/60</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1.9199999999999998E-2</v>
       </c>
       <c r="X24" s="1">
-        <f>Q24/1000000 *20 * 365</f>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>50457.600000000006</v>
       </c>
       <c r="Y24" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9.6000000000000016E-2</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1">
-        <v>2000</v>
+        <v>7100</v>
       </c>
       <c r="D25" s="11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F25" s="5">
-        <v>32</v>
+        <v>256</v>
       </c>
       <c r="G25" s="5">
-        <v>512</v>
+        <v>819</v>
+      </c>
+      <c r="H25" s="5">
+        <v>114</v>
       </c>
       <c r="I25" s="5">
         <v>300</v>
       </c>
+      <c r="J25" s="5">
+        <v>80</v>
+      </c>
       <c r="L25" s="2">
-        <f t="shared" si="18"/>
-        <v>62.5</v>
+        <f t="shared" ref="L25:N28" si="19">$C25/F25</f>
+        <v>27.734375</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" si="18"/>
-        <v>3.90625</v>
-      </c>
-      <c r="N25" s="2" t="e">
-        <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O25" s="2" t="e">
+        <f t="shared" si="19"/>
+        <v>8.6691086691086685</v>
+      </c>
+      <c r="N25" s="2">
+        <f t="shared" si="19"/>
+        <v>62.280701754385966</v>
+      </c>
+      <c r="O25" s="2">
         <f>$C25/J25</f>
-        <v>#DIV/0!</v>
+        <v>88.75</v>
       </c>
       <c r="Q25" s="6">
         <f>J25*86400</f>
-        <v>0</v>
-      </c>
-      <c r="R25" s="4" t="e">
+        <v>6912000</v>
+      </c>
+      <c r="R25" s="4">
         <f>I25/J25</f>
-        <v>#DIV/0!</v>
+        <v>3.75</v>
       </c>
       <c r="T25" s="1">
         <f>Q25/1000000 *2 * 365</f>
-        <v>0</v>
+        <v>5045.76</v>
       </c>
       <c r="U25" s="1">
-        <f>T25/365/24/60</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>9.5999999999999992E-3</v>
       </c>
       <c r="V25" s="1">
         <f>Q25/1000000 *4 * 365</f>
-        <v>0</v>
+        <v>10091.52</v>
       </c>
       <c r="W25" s="1">
-        <f>V25/365/24/60</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1.9199999999999998E-2</v>
       </c>
       <c r="X25" s="1">
         <f>Q25/1000000 *20 * 365</f>
-        <v>0</v>
+        <v>50457.600000000006</v>
       </c>
       <c r="Y25" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>9.6000000000000016E-2</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C26" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1500</v>
+      </c>
       <c r="D26" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="5">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G26" s="5">
-        <v>0</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0</v>
+        <v>512</v>
       </c>
       <c r="I26" s="5">
-        <v>0</v>
-      </c>
-      <c r="J26" s="5">
-        <v>0</v>
-      </c>
-      <c r="L26" s="2" t="e">
-        <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M26" s="2" t="e">
-        <f t="shared" si="18"/>
-        <v>#DIV/0!</v>
+        <v>300</v>
+      </c>
+      <c r="L26" s="2">
+        <f t="shared" si="19"/>
+        <v>53.571428571428569</v>
+      </c>
+      <c r="M26" s="2">
+        <f t="shared" si="19"/>
+        <v>2.9296875</v>
       </c>
       <c r="N26" s="2" t="e">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O26" s="2" t="e">
@@ -2794,13 +2808,159 @@
         <v>0</v>
       </c>
       <c r="Y26" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D27" s="11">
+        <v>1</v>
+      </c>
+      <c r="F27" s="5">
+        <v>32</v>
+      </c>
+      <c r="G27" s="5">
+        <v>512</v>
+      </c>
+      <c r="I27" s="5">
+        <v>300</v>
+      </c>
+      <c r="L27" s="2">
+        <f t="shared" si="19"/>
+        <v>62.5</v>
+      </c>
+      <c r="M27" s="2">
+        <f t="shared" si="19"/>
+        <v>3.90625</v>
+      </c>
+      <c r="N27" s="2" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O27" s="2" t="e">
+        <f>$C27/J27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q27" s="6">
+        <f>J27*86400</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="4" t="e">
+        <f>I27/J27</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T27" s="1">
+        <f>Q27/1000000 *2 * 365</f>
+        <v>0</v>
+      </c>
+      <c r="U27" s="1">
+        <f>T27/365/24/60</f>
+        <v>0</v>
+      </c>
+      <c r="V27" s="1">
+        <f>Q27/1000000 *4 * 365</f>
+        <v>0</v>
+      </c>
+      <c r="W27" s="1">
+        <f>V27/365/24/60</f>
+        <v>0</v>
+      </c>
+      <c r="X27" s="1">
+        <f>Q27/1000000 *20 * 365</f>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="11">
+        <v>0</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M28" s="2" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N28" s="2" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O28" s="2" t="e">
+        <f>$C28/J28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q28" s="6">
+        <f>J28*86400</f>
+        <v>0</v>
+      </c>
+      <c r="R28" s="4" t="e">
+        <f>I28/J28</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T28" s="1">
+        <f>Q28/1000000 *2 * 365</f>
+        <v>0</v>
+      </c>
+      <c r="U28" s="1">
+        <f>T28/365/24/60</f>
+        <v>0</v>
+      </c>
+      <c r="V28" s="1">
+        <f>Q28/1000000 *4 * 365</f>
+        <v>0</v>
+      </c>
+      <c r="W28" s="1">
+        <f>V28/365/24/60</f>
+        <v>0</v>
+      </c>
+      <c r="X28" s="1">
+        <f>Q28/1000000 *20 * 365</f>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="1">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C2:D26">
+  <conditionalFormatting sqref="C2:D28">
     <cfRule type="colorScale" priority="92">
       <colorScale>
         <cfvo type="min"/>
@@ -2812,7 +2972,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="D2:D28">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -2824,7 +2984,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F26">
+  <conditionalFormatting sqref="F2:F28">
     <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
@@ -2836,7 +2996,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G26">
+  <conditionalFormatting sqref="G2:G28">
     <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
@@ -2848,7 +3008,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H26">
+  <conditionalFormatting sqref="H2:H28">
     <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
@@ -2860,7 +3020,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I26">
+  <conditionalFormatting sqref="I2:I28">
     <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
@@ -2872,7 +3032,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J26">
+  <conditionalFormatting sqref="J2:J28">
     <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="min"/>
@@ -2884,7 +3044,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L26">
+  <conditionalFormatting sqref="L2:L28">
     <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
@@ -2896,7 +3056,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M26">
+  <conditionalFormatting sqref="M2:M28">
     <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
@@ -2908,7 +3068,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N26">
+  <conditionalFormatting sqref="N2:N28">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -2920,7 +3080,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O26">
+  <conditionalFormatting sqref="O2:O28">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -2932,7 +3092,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q26">
+  <conditionalFormatting sqref="Q2:Q28">
     <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
@@ -2944,7 +3104,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R26">
+  <conditionalFormatting sqref="R2:R28">
     <cfRule type="colorScale" priority="68">
       <colorScale>
         <cfvo type="min"/>
@@ -2956,7 +3116,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T26">
+  <conditionalFormatting sqref="T2:T28">
     <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="min"/>
@@ -2968,7 +3128,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U2:U26">
+  <conditionalFormatting sqref="U2:U28">
     <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="min"/>
@@ -2980,7 +3140,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V2:V26">
+  <conditionalFormatting sqref="V2:V28">
     <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min"/>
@@ -2992,7 +3152,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W2:W26">
+  <conditionalFormatting sqref="W2:W28">
     <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="min"/>
@@ -3004,7 +3164,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X2:X26">
+  <conditionalFormatting sqref="X2:X28">
     <cfRule type="colorScale" priority="88">
       <colorScale>
         <cfvo type="min"/>
@@ -3016,7 +3176,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Y2:Y26">
+  <conditionalFormatting sqref="Y2:Y28">
     <cfRule type="colorScale" priority="90">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>